<commit_message>
CHANGE: fill_pdf function complete, slicing dict per each pdf page
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -551,7 +551,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>09.03.21</t>
+          <t>10.03.21</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -654,7 +654,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>09.03.21</t>
+          <t>10.03.21</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -757,7 +757,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>09.03.21</t>
+          <t>10.03.21</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -860,7 +860,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>09.03.21</t>
+          <t>10.03.21</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -963,7 +963,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>09.03.21</t>
+          <t>10.03.21</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -1066,7 +1066,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>09.03.21</t>
+          <t>10.03.21</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -1169,7 +1169,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>09.03.21</t>
+          <t>10.03.21</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -1272,7 +1272,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>09.03.21</t>
+          <t>10.03.21</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -1375,7 +1375,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>09.03.21</t>
+          <t>10.03.21</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -1478,7 +1478,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>09.03.21</t>
+          <t>10.03.21</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -1581,7 +1581,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>09.03.21</t>
+          <t>10.03.21</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -1684,7 +1684,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>09.03.21</t>
+          <t>10.03.21</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">

</xml_diff>

<commit_message>
FIX: change dict keys for each pdf page:value
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -551,7 +551,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>10.03.21</t>
+          <t>11.03.21</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -654,7 +654,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>10.03.21</t>
+          <t>11.03.21</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -757,7 +757,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>10.03.21</t>
+          <t>11.03.21</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -860,7 +860,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>10.03.21</t>
+          <t>11.03.21</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -963,7 +963,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>10.03.21</t>
+          <t>11.03.21</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -1066,7 +1066,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>10.03.21</t>
+          <t>11.03.21</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -1169,7 +1169,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>10.03.21</t>
+          <t>11.03.21</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -1272,7 +1272,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>10.03.21</t>
+          <t>11.03.21</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -1375,7 +1375,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>10.03.21</t>
+          <t>11.03.21</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -1478,7 +1478,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>10.03.21</t>
+          <t>11.03.21</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -1581,7 +1581,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>10.03.21</t>
+          <t>11.03.21</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -1684,7 +1684,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>10.03.21</t>
+          <t>11.03.21</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">

</xml_diff>